<commit_message>
removed class for background task
</commit_message>
<xml_diff>
--- a/warnings.xlsx
+++ b/warnings.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15440" windowWidth="28800" xWindow="27800" yWindow="2540"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15435" windowWidth="28800" xWindow="1950" yWindow="1950"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -381,10 +381,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -425,31 +425,6 @@
           <t>TheDankestPutin#1389</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>test01</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>test02</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>No reason given.</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>No reason given.</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>No reason given.</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">

</xml_diff>